<commit_message>
Correção dos 22 e 23
</commit_message>
<xml_diff>
--- a/Artefatos/23. Matriz de Rastreabilidade.xlsx
+++ b/Artefatos/23. Matriz de Rastreabilidade.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22913"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7D0EDBDB-10F6-442B-BC2C-959F452C16CF}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1338AC68-FF7F-4722-9A07-7F87F2DCC40F}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>#</t>
   </si>
@@ -36,46 +36,133 @@
     <t>Requisistos</t>
   </si>
   <si>
-    <t xml:space="preserve">Notas físcais </t>
-  </si>
-  <si>
-    <t>SSS01,SSS14</t>
-  </si>
-  <si>
-    <t>Pedidos de orçamento</t>
-  </si>
-  <si>
-    <t>SSS16</t>
-  </si>
-  <si>
-    <t>Modificação do pedido</t>
-  </si>
-  <si>
-    <t>SSS12</t>
-  </si>
-  <si>
-    <t>Pedidos devolvidos</t>
-  </si>
-  <si>
-    <t>SSS01,SSS10</t>
-  </si>
-  <si>
-    <t>Retirada de mercadorias</t>
-  </si>
-  <si>
-    <t>SSS06</t>
-  </si>
-  <si>
-    <t>Atualização do sistema</t>
-  </si>
-  <si>
-    <t>SSS02,SSS03,SSS15,SSS11</t>
-  </si>
-  <si>
-    <t>Auteração de Pedido</t>
-  </si>
-  <si>
-    <t>SSS13,SSS03</t>
+    <t xml:space="preserve">Sistema Web </t>
+  </si>
+  <si>
+    <t>SSS15,SSS13 ,SSS08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestão de perfil do usuário </t>
+  </si>
+  <si>
+    <t>SSS15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro de venda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSS03,SSS04,SSS05,SSS12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realização  de orçamento </t>
+  </si>
+  <si>
+    <t>SSS17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recebimento de  mercadorias </t>
+  </si>
+  <si>
+    <t>SSS01,SSS02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contagem do estoque  </t>
+  </si>
+  <si>
+    <t>SSS02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendas de produtos </t>
+  </si>
+  <si>
+    <t>SSS18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trocas produtos </t>
+  </si>
+  <si>
+    <t>SSS10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devolução de mercadoria </t>
+  </si>
+  <si>
+    <t>SSS19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catalogo de produtos </t>
+  </si>
+  <si>
+    <t>SSS21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avisos via telefone </t>
+  </si>
+  <si>
+    <t>SSS22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divulgação da marca </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divulgação de produtos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notificação de venda  </t>
+  </si>
+  <si>
+    <t>SSS23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aprovação de orçamento do material </t>
+  </si>
+  <si>
+    <t>SSS24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulta de preço </t>
+  </si>
+  <si>
+    <t>SSS25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alteração de prazo  </t>
+  </si>
+  <si>
+    <t>SSS13,SSS17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar material do produto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relatório de venda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSS11 </t>
+  </si>
+  <si>
+    <t>Inventário de produtos</t>
+  </si>
+  <si>
+    <t>SSS20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alteração de preço </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promoção de vendas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avisos via email </t>
+  </si>
+  <si>
+    <t>SSS07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avisos via whatsapp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avisos via facebook </t>
   </si>
 </sst>
 </file>
@@ -150,8 +237,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{179CFD4A-FBB7-4A58-B702-E635E58840FF}" name="Tabela1" displayName="Tabela1" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{084F0CC2-E910-4FB0-AAC0-25D7F9C01AD4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{179CFD4A-FBB7-4A58-B702-E635E58840FF}" name="Tabela1" displayName="Tabela1" ref="A1:C26" totalsRowShown="0">
+  <autoFilter ref="A1:C26" xr:uid="{084F0CC2-E910-4FB0-AAC0-25D7F9C01AD4}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2D401429-DAF4-4891-B791-DC8FB8031649}" name="#" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6B98524C-9BCD-4B48-8DCA-3A95C966C3A5}" name="Características"/>
@@ -458,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -484,7 +571,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -495,7 +582,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -506,7 +593,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -517,7 +604,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -528,7 +615,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -539,7 +626,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -550,7 +637,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -559,8 +646,224 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="12" spans="1:3">
-      <c r="C12" s="3"/>
+      <c r="A12" s="2">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>